<commit_message>
Fixing Excel SCD0197 - SCD0218 and Delete Unclear Report
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0197 - Penyelia SRM Mengakses Menu Report - Menu Product Holding Ratio - Report.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0197 - Penyelia SRM Mengakses Menu Report - Menu Product Holding Ratio - Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BEC7BB2-210A-4EF3-8B14-EEF56C08569D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C12FFE-7944-4BB2-B102-797D8FF74620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1365" yWindow="3645" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCD0197" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>SIDEBAR_MENU</t>
   </si>
@@ -92,76 +92,34 @@
     <t>TEXT5</t>
   </si>
   <si>
-    <t>QUERY1</t>
-  </si>
-  <si>
-    <t>QUERY2</t>
-  </si>
-  <si>
-    <t>QUERY3</t>
-  </si>
-  <si>
-    <t>EXPL_QUERY1</t>
-  </si>
-  <si>
-    <t>EXPL_QUERY2</t>
-  </si>
-  <si>
-    <t>EXPL_QUERY3</t>
-  </si>
-  <si>
-    <t>USER_DB</t>
-  </si>
-  <si>
-    <t>PASSWORD_DB</t>
-  </si>
-  <si>
-    <t>HOSTNAME</t>
-  </si>
-  <si>
-    <t>sa</t>
-  </si>
-  <si>
-    <t>4eFfEJAA!</t>
-  </si>
-  <si>
-    <t>192.168.232.6</t>
-  </si>
-  <si>
     <t>Februari</t>
   </si>
   <si>
-    <t>1. login digisales portal dengan pimpinan wilayah 18994
+    <t>Penyelia SRM mengakses menu: Report Menu - Product Holding Ratio - Report</t>
+  </si>
+  <si>
+    <t>Penyelia SRM</t>
+  </si>
+  <si>
+    <t>DGS-212</t>
+  </si>
+  <si>
+    <t>9188251160</t>
+  </si>
+  <si>
+    <t>1. login digisales portal dengan penyelia SRM 37400
 2. buka menu product holding
-3. isi field npp sales sendiri dengan 39798, dengan field tahun, bulan dan jenis nasabah (tahun 2022 bulan februari) 
+3. isi field npp sales sendiri dengan 39798, dengan field tahun, bulan, dan CIF  (tahun 2022 bulan februari) 
 4. klik generate
 5. data muncul
 7. klik export file, pilih salah jenis xls atau xlsx
 8. data report excel berhasil terdownload dan dapat dilihat</t>
   </si>
   <si>
-    <t>Penyelia SRM mengakses menu: Report Menu - Product Holding Ratio - Report</t>
-  </si>
-  <si>
-    <t>Penyelia SRM</t>
-  </si>
-  <si>
-    <t>SELECT * FROM DigisalesNew..Tbl_Pegawai WHERE SalesTypeId='20' and LastLogin IS NOT NULL</t>
-  </si>
-  <si>
-    <t>DGS-212</t>
-  </si>
-  <si>
-    <t>1. login digisales portal dengan penyelia SRM 37400
-2. buka menu product holding
-3. isi field npp sales sendiri dengan 32587, dengan field tahun, bulan, dan CIF  (tahun 2022 bulan februari) 
-4. klik generate
-5. data muncul
-7. klik export file, pilih salah jenis xls atau xlsx
-8. data report excel berhasil terdownload dan dapat dilihat</t>
-  </si>
-  <si>
-    <t>9188251160</t>
+    <t xml:space="preserve"> - Hanya dapat memilih Sales tipe SRM 
+ - Berhasil menampilkan data sesuai dengan keyword yang di tentukan
+ - Berhasil meng-export data sesuai dengan keyword yang di tentukan
+ - Excel sesuai dengan format yang di lampirkan pada BSDD</t>
   </si>
 </sst>
 </file>
@@ -215,38 +173,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -557,7 +511,7 @@
   <dimension ref="A1:Z6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,7 +523,7 @@
     <col min="5" max="5" width="37.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -638,58 +592,31 @@
       <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="X1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>28</v>
-      </c>
     </row>
-    <row r="2" spans="1:26" ht="153" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="102" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="4">
         <v>37400</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>15</v>
@@ -701,63 +628,52 @@
         <v>2022</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="P2" s="5"/>
       <c r="Q2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="U2" s="10" t="str">
-        <f>"Pembuktian Sales yang ada pada User " &amp; F2</f>
-        <v>Pembuktian Sales yang ada pada User 37400</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z2" s="10" t="s">
-        <v>31</v>
-      </c>
+      <c r="R2" s="6"/>
+      <c r="U2" s="7"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="7"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B3" s="6"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="3"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-      <c r="I3" s="7"/>
+      <c r="I3" s="8"/>
       <c r="Q3" s="5"/>
-      <c r="R3" s="8"/>
+      <c r="R3" s="9"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="3"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="I4" s="7"/>
+      <c r="I4" s="8"/>
       <c r="Q4" s="5"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="9"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
-      <c r="F5" s="3"/>
+      <c r="B5" s="2"/>
+      <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-      <c r="F6" s="3"/>
+      <c r="B6" s="2"/>
+      <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
   </sheetData>

</xml_diff>